<commit_message>
modify paper under the teacher's advices
</commit_message>
<xml_diff>
--- a/Mypaper/tables/4.5风险因素概率统计分析.xlsx
+++ b/Mypaper/tables/4.5风险因素概率统计分析.xlsx
@@ -37,13 +37,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>需求不明确风险因素R</t>
     </r>
     <r>
@@ -70,13 +63,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>需求蔓延风险因素R</t>
     </r>
     <r>
@@ -103,13 +89,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>需求持续变更风险因素R</t>
     </r>
     <r>
@@ -727,6 +706,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>中国Android被取消授权风险因素R</t>
     </r>
     <r>
@@ -813,8 +799,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -852,52 +838,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -906,16 +846,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -931,9 +870,54 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -946,8 +930,24 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -963,20 +963,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1014,13 +1000,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,169 +1054,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1223,15 +1209,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1243,6 +1220,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1264,35 +1265,20 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1328,10 +1314,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1340,16 +1326,16 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1358,115 +1344,115 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1837,14 +1823,17 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:F25"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-    <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="8.75" customWidth="1"/>
+    <col min="1" max="1" width="38.075" customWidth="1"/>
+    <col min="2" max="2" width="7.01666666666667" customWidth="1"/>
+    <col min="3" max="3" width="4.80833333333333" customWidth="1"/>
+    <col min="4" max="4" width="4.9" customWidth="1"/>
+    <col min="5" max="5" width="3.84166666666667" customWidth="1"/>
+    <col min="6" max="6" width="5.95833333333333" customWidth="1"/>
     <col min="7" max="7" width="14.375" customWidth="1"/>
     <col min="9" max="9" width="12.625"/>
   </cols>
@@ -1892,15 +1881,15 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f>SUM(B2:F2)</f>
+        <f t="shared" ref="G2:G24" si="0">SUM(B2:F2)</f>
         <v>242</v>
       </c>
       <c r="H2">
-        <f>SUM(B2*0.9,C2*0.7,D2*0.5,E2*0.3,F2*0.1)</f>
+        <f t="shared" ref="H2:H24" si="1">SUM(B2*0.9,C2*0.7,D2*0.5,E2*0.3,F2*0.1)</f>
         <v>210</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(H2/242)</f>
+        <f t="shared" ref="I2:I24" si="2">AVERAGE(H2/242)</f>
         <v>0.867768595041322</v>
       </c>
       <c r="J2">
@@ -1927,15 +1916,15 @@
         <v>5</v>
       </c>
       <c r="G3">
-        <f>SUM(B3:F3)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H3">
-        <f>SUM(B3*0.9,C3*0.7,D3*0.5,E3*0.3,F3*0.1)</f>
+        <f t="shared" si="1"/>
         <v>181.6</v>
       </c>
       <c r="I3">
-        <f>AVERAGE(H3/242)</f>
+        <f t="shared" si="2"/>
         <v>0.750413223140496</v>
       </c>
       <c r="J3">
@@ -1962,15 +1951,15 @@
         <v>5</v>
       </c>
       <c r="G4">
-        <f>SUM(B4:F4)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H4">
-        <f>SUM(B4*0.9,C4*0.7,D4*0.5,E4*0.3,F4*0.1)</f>
+        <f t="shared" si="1"/>
         <v>193.6</v>
       </c>
       <c r="I4">
-        <f>AVERAGE(H4/242)</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="J4">
@@ -1997,15 +1986,15 @@
         <v>21</v>
       </c>
       <c r="G5">
-        <f>SUM(B5:F5)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H5">
-        <f>SUM(B5*0.9,C5*0.7,D5*0.5,E5*0.3,F5*0.1)</f>
+        <f t="shared" si="1"/>
         <v>85.2</v>
       </c>
       <c r="I5">
-        <f>AVERAGE(H5/242)</f>
+        <f t="shared" si="2"/>
         <v>0.352066115702479</v>
       </c>
       <c r="J5">
@@ -2032,15 +2021,15 @@
         <v>12</v>
       </c>
       <c r="G6">
-        <f>SUM(B6:F6)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H6">
-        <f>SUM(B6*0.9,C6*0.7,D6*0.5,E6*0.3,F6*0.1)</f>
+        <f t="shared" si="1"/>
         <v>94.6</v>
       </c>
       <c r="I6">
-        <f>AVERAGE(H6/242)</f>
+        <f t="shared" si="2"/>
         <v>0.390909090909091</v>
       </c>
       <c r="J6">
@@ -2067,15 +2056,15 @@
         <v>102</v>
       </c>
       <c r="G7">
-        <f>SUM(B7:F7)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H7">
-        <f>SUM(B7*0.9,C7*0.7,D7*0.5,E7*0.3,F7*0.1)</f>
+        <f t="shared" si="1"/>
         <v>63.6</v>
       </c>
       <c r="I7">
-        <f>AVERAGE(H7/242)</f>
+        <f t="shared" si="2"/>
         <v>0.262809917355372</v>
       </c>
       <c r="J7">
@@ -2102,15 +2091,15 @@
         <v>88</v>
       </c>
       <c r="G8">
-        <f>SUM(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H8">
-        <f>SUM(B8*0.9,C8*0.7,D8*0.5,E8*0.3,F8*0.1)</f>
+        <f t="shared" si="1"/>
         <v>66.2</v>
       </c>
       <c r="I8">
-        <f>AVERAGE(H8/242)</f>
+        <f t="shared" si="2"/>
         <v>0.273553719008264</v>
       </c>
       <c r="J8">
@@ -2137,15 +2126,15 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <f>SUM(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H9">
-        <f>SUM(B9*0.9,C9*0.7,D9*0.5,E9*0.3,F9*0.1)</f>
+        <f t="shared" si="1"/>
         <v>193.6</v>
       </c>
       <c r="I9">
-        <f>AVERAGE(H9/242)</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="J9">
@@ -2172,15 +2161,15 @@
         <v>2</v>
       </c>
       <c r="G10">
-        <f>SUM(B10:F10)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H10">
-        <f>SUM(B10*0.9,C10*0.7,D10*0.5,E10*0.3,F10*0.1)</f>
+        <f t="shared" si="1"/>
         <v>132.6</v>
       </c>
       <c r="I10">
-        <f>AVERAGE(H10/242)</f>
+        <f t="shared" si="2"/>
         <v>0.547933884297521</v>
       </c>
       <c r="J10">
@@ -2207,15 +2196,15 @@
         <v>12</v>
       </c>
       <c r="G11">
-        <f>SUM(B11:F11)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H11">
-        <f>SUM(B11*0.9,C11*0.7,D11*0.5,E11*0.3,F11*0.1)</f>
+        <f t="shared" si="1"/>
         <v>141.8</v>
       </c>
       <c r="I11">
-        <f>AVERAGE(H11/242)</f>
+        <f t="shared" si="2"/>
         <v>0.58595041322314</v>
       </c>
       <c r="J11">
@@ -2242,15 +2231,15 @@
         <v>9</v>
       </c>
       <c r="G12">
-        <f>SUM(B12:F12)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H12">
-        <f>SUM(B12*0.9,C12*0.7,D12*0.5,E12*0.3,F12*0.1)</f>
+        <f t="shared" si="1"/>
         <v>153.8</v>
       </c>
       <c r="I12">
-        <f>AVERAGE(H12/242)</f>
+        <f t="shared" si="2"/>
         <v>0.635537190082645</v>
       </c>
       <c r="J12">
@@ -2277,15 +2266,15 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <f>SUM(B13:F13)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H13">
-        <f>SUM(B13*0.9,C13*0.7,D13*0.5,E13*0.3,F13*0.1)</f>
+        <f t="shared" si="1"/>
         <v>213.2</v>
       </c>
       <c r="I13">
-        <f>AVERAGE(H13/242)</f>
+        <f t="shared" si="2"/>
         <v>0.88099173553719</v>
       </c>
       <c r="J13">
@@ -2312,15 +2301,15 @@
         <v>10</v>
       </c>
       <c r="G14">
-        <f>SUM(B14:F14)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H14">
-        <f>SUM(B14*0.9,C14*0.7,D14*0.5,E14*0.3,F14*0.1)</f>
+        <f t="shared" si="1"/>
         <v>133</v>
       </c>
       <c r="I14">
-        <f>AVERAGE(H14/242)</f>
+        <f t="shared" si="2"/>
         <v>0.549586776859504</v>
       </c>
       <c r="J14">
@@ -2347,15 +2336,15 @@
         <v>2</v>
       </c>
       <c r="G15">
-        <f>SUM(B15:F15)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H15">
-        <f>SUM(B15*0.9,C15*0.7,D15*0.5,E15*0.3,F15*0.1)</f>
+        <f t="shared" si="1"/>
         <v>195.4</v>
       </c>
       <c r="I15">
-        <f>AVERAGE(H15/242)</f>
+        <f t="shared" si="2"/>
         <v>0.807438016528926</v>
       </c>
       <c r="J15">
@@ -2382,15 +2371,15 @@
         <v>12</v>
       </c>
       <c r="G16">
-        <f>SUM(B16:F16)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H16">
-        <f>SUM(B16*0.9,C16*0.7,D16*0.5,E16*0.3,F16*0.1)</f>
+        <f t="shared" si="1"/>
         <v>122.4</v>
       </c>
       <c r="I16">
-        <f>AVERAGE(H16/242)</f>
+        <f t="shared" si="2"/>
         <v>0.505785123966942</v>
       </c>
       <c r="J16">
@@ -2417,15 +2406,15 @@
         <v>43</v>
       </c>
       <c r="G17">
-        <f>SUM(B17:F17)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H17">
-        <f>SUM(B17*0.9,C17*0.7,D17*0.5,E17*0.3,F17*0.1)</f>
+        <f t="shared" si="1"/>
         <v>80.4</v>
       </c>
       <c r="I17">
-        <f>AVERAGE(H17/242)</f>
+        <f t="shared" si="2"/>
         <v>0.332231404958678</v>
       </c>
       <c r="J17">
@@ -2452,15 +2441,15 @@
         <v>53</v>
       </c>
       <c r="G18">
-        <f>SUM(B18:F18)</f>
+        <f t="shared" si="0"/>
         <v>241</v>
       </c>
       <c r="H18">
-        <f>SUM(B18*0.9,C18*0.7,D18*0.5,E18*0.3,F18*0.1)</f>
+        <f t="shared" si="1"/>
         <v>76.9</v>
       </c>
       <c r="I18">
-        <f>AVERAGE(H18/242)</f>
+        <f t="shared" si="2"/>
         <v>0.317768595041322</v>
       </c>
       <c r="J18">
@@ -2487,15 +2476,15 @@
         <v>66</v>
       </c>
       <c r="G19">
-        <f>SUM(B19:F19)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H19">
-        <f>SUM(B19*0.9,C19*0.7,D19*0.5,E19*0.3,F19*0.1)</f>
+        <f t="shared" si="1"/>
         <v>78.4</v>
       </c>
       <c r="I19">
-        <f>AVERAGE(H19/242)</f>
+        <f t="shared" si="2"/>
         <v>0.32396694214876</v>
       </c>
       <c r="J19">
@@ -2522,15 +2511,15 @@
         <v>21</v>
       </c>
       <c r="G20">
-        <f>SUM(B20:F20)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H20">
-        <f>SUM(B20*0.9,C20*0.7,D20*0.5,E20*0.3,F20*0.1)</f>
+        <f t="shared" si="1"/>
         <v>113.6</v>
       </c>
       <c r="I20">
-        <f>AVERAGE(H20/242)</f>
+        <f t="shared" si="2"/>
         <v>0.469421487603306</v>
       </c>
       <c r="J20">
@@ -2557,15 +2546,15 @@
         <v>70</v>
       </c>
       <c r="G21">
-        <f>SUM(B21:F21)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H21">
-        <f>SUM(B21*0.9,C21*0.7,D21*0.5,E21*0.3,F21*0.1)</f>
+        <f t="shared" si="1"/>
         <v>83.2</v>
       </c>
       <c r="I21">
-        <f>AVERAGE(H21/242)</f>
+        <f t="shared" si="2"/>
         <v>0.343801652892562</v>
       </c>
       <c r="J21">
@@ -2592,15 +2581,15 @@
         <v>111</v>
       </c>
       <c r="G22">
-        <f>SUM(B22:F22)</f>
+        <f t="shared" si="0"/>
         <v>240</v>
       </c>
       <c r="H22">
-        <f>SUM(B22*0.9,C22*0.7,D22*0.5,E22*0.3,F22*0.1)</f>
+        <f t="shared" si="1"/>
         <v>66</v>
       </c>
       <c r="I22">
-        <f>AVERAGE(H22/242)</f>
+        <f t="shared" si="2"/>
         <v>0.272727272727273</v>
       </c>
       <c r="J22">
@@ -2627,15 +2616,15 @@
         <v>216</v>
       </c>
       <c r="G23">
-        <f>SUM(B23:F23)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H23">
-        <f>SUM(B23*0.9,C23*0.7,D23*0.5,E23*0.3,F23*0.1)</f>
+        <f t="shared" si="1"/>
         <v>30.2</v>
       </c>
       <c r="I23">
-        <f>AVERAGE(H23/242)</f>
+        <f t="shared" si="2"/>
         <v>0.124793388429752</v>
       </c>
       <c r="J23">
@@ -2646,7 +2635,9 @@
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
       <c r="C24" s="1">
         <v>1</v>
       </c>
@@ -2660,15 +2651,15 @@
         <v>179</v>
       </c>
       <c r="G24">
-        <f>SUM(B24:F24)</f>
+        <f t="shared" si="0"/>
         <v>242</v>
       </c>
       <c r="H24">
-        <f>SUM(B24*0.9,C24*0.7,D24*0.5,E24*0.3,F24*0.1)</f>
+        <f t="shared" si="1"/>
         <v>40.6</v>
       </c>
       <c r="I24">
-        <f>AVERAGE(H24/242)</f>
+        <f t="shared" si="2"/>
         <v>0.167768595041322</v>
       </c>
       <c r="J24">

</xml_diff>